<commit_message>
Update datatables populate into function
</commit_message>
<xml_diff>
--- a/TeachingAssignmentManagement/Uploads/CNTT UIS-ThoiKhoaBieu_TieuChuan_Null.xlsx
+++ b/TeachingAssignmentManagement/Uploads/CNTT UIS-ThoiKhoaBieu_TieuChuan_Null.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duy94\Downloads\Excel dữ liệu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971503A1-899A-4844-870A-6AE372A7BEA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1F5ADF1-12EA-41A1-9251-85D34A7B7B5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6061,10 +6061,10 @@
   <dimension ref="A1:AF312"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E288" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P296" sqref="P296"/>
+      <selection pane="bottomRight" activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Update demo file for import timetable
Related Work Items: #1521
</commit_message>
<xml_diff>
--- a/TeachingAssignmentManagement/Uploads/CNTT UIS-ThoiKhoaBieu_TieuChuan_Null.xlsx
+++ b/TeachingAssignmentManagement/Uploads/CNTT UIS-ThoiKhoaBieu_TieuChuan_Null.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duy94\Downloads\Excel dữ liệu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1F5ADF1-12EA-41A1-9251-85D34A7B7B5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91B42D8-D879-4EAF-9F57-DD0450A3C023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6064,13 +6064,13 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L7" sqref="L7"/>
+      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.44140625" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="1" max="1" width="23.44140625" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="23.33203125" customWidth="1"/>
     <col min="4" max="4" width="30.88671875" customWidth="1"/>
     <col min="5" max="5" width="5.44140625" customWidth="1"/>

</xml_diff>

<commit_message>
Catch error row when import
Related Work Items: #1521
</commit_message>
<xml_diff>
--- a/TeachingAssignmentManagement/Uploads/CNTT UIS-ThoiKhoaBieu_TieuChuan_Null.xlsx
+++ b/TeachingAssignmentManagement/Uploads/CNTT UIS-ThoiKhoaBieu_TieuChuan_Null.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duy94\Downloads\Excel dữ liệu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91B42D8-D879-4EAF-9F57-DD0450A3C023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C28CB5-D653-47C4-B677-AD3FB35BD99F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9051" uniqueCount="768">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9050" uniqueCount="768">
   <si>
     <t>MaGocLHP</t>
   </si>
@@ -6064,7 +6064,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6194,7 +6194,7 @@
         <v>31</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>32</v>
@@ -7113,9 +7113,7 @@
       <c r="B12" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>89</v>
-      </c>
+      <c r="C12" s="8"/>
       <c r="D12" s="8" t="s">
         <v>32</v>
       </c>

</xml_diff>